<commit_message>
Grace 4th updates on 0804
</commit_message>
<xml_diff>
--- a/SDG Financing Simplified model (Egypt)/v4_commented and cleaned - for calibration/auxiliary/datainput_arg.xlsx
+++ b/SDG Financing Simplified model (Egypt)/v4_commented and cleaned - for calibration/auxiliary/datainput_arg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="123">
   <si>
     <t>male</t>
   </si>
@@ -9250,14 +9250,210 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.376799063321304</v>
+      </c>
+      <c r="C2">
+        <v>0.363098589278724</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.37622959934274</v>
+      </c>
+      <c r="C3">
+        <v>0.36259922788128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.373923065099844</v>
+      </c>
+      <c r="C4">
+        <v>0.360422582568516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.371616530856948</v>
+      </c>
+      <c r="C5">
+        <v>0.358245937255752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0.369309996614052</v>
+      </c>
+      <c r="C6">
+        <v>0.356069291942988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.367003462371156</v>
+      </c>
+      <c r="C7">
+        <v>0.353892646630224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.36391719422646</v>
+      </c>
+      <c r="C8">
+        <v>0.3487800287966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.362666749976688</v>
+      </c>
+      <c r="C9">
+        <v>0.34773916379756</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.361416305726916</v>
+      </c>
+      <c r="C10">
+        <v>0.34669829879852</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0.309666987090648</v>
+      </c>
+      <c r="C11">
+        <v>0.326896685568684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0.308591867694924</v>
+      </c>
+      <c r="C12">
+        <v>0.325912314092652</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.3075167482992</v>
+      </c>
+      <c r="C13">
+        <v>0.32492794261662</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0.34216068404</v>
+      </c>
+      <c r="C14">
+        <v>0.33114861754</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0.34074718408</v>
+      </c>
+      <c r="C15">
+        <v>0.33019060498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>0.33933368412</v>
+      </c>
+      <c r="C16">
+        <v>0.32923259242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>0.33792018416</v>
+      </c>
+      <c r="C17">
+        <v>0.32827457986</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>0.3365066842</v>
+      </c>
+      <c r="C18">
+        <v>0.3273165673</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>